<commit_message>
Change Name of Output
</commit_message>
<xml_diff>
--- a/output/Scores Week 1.xlsx
+++ b/output/Scores Week 1.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:AZ20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -448,42 +448,257 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Brandon</t>
+          <t>Annalise B.</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Ingvild</t>
+          <t>Austin K.</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Dave</t>
+          <t>Barbara T.</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Carson</t>
+          <t>Brad S.</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Inge</t>
+          <t>Brady M.</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Lisbeth</t>
+          <t>Brandon T.</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>Sander</t>
+          <t>Brian M.</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>Stian</t>
+          <t>Calvin M.</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Carlos G.</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Carrisa K.</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Carson T.</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Colton S.</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Curtis K.</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Curtis M.</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>Dave T.</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>Dean M.</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>Diana V.</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>Dino V.</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>Elliot N.</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>Jeremiah C.</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>Jerome D.</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>Joe V.</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>John Mak.</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>John Mc.</t>
+        </is>
+      </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>Jordon</t>
+        </is>
+      </c>
+      <c r="AA1" s="1" t="inlineStr">
+        <is>
+          <t>Kelly C.</t>
+        </is>
+      </c>
+      <c r="AB1" s="1" t="inlineStr">
+        <is>
+          <t>Kevin J. #1</t>
+        </is>
+      </c>
+      <c r="AC1" s="1" t="inlineStr">
+        <is>
+          <t>Kevin J. #2</t>
+        </is>
+      </c>
+      <c r="AD1" s="1" t="inlineStr">
+        <is>
+          <t>Kevin M.</t>
+        </is>
+      </c>
+      <c r="AE1" s="1" t="inlineStr">
+        <is>
+          <t>Kyle K.</t>
+        </is>
+      </c>
+      <c r="AF1" s="1" t="inlineStr">
+        <is>
+          <t>Kyle P.</t>
+        </is>
+      </c>
+      <c r="AG1" s="1" t="inlineStr">
+        <is>
+          <t>Les D.</t>
+        </is>
+      </c>
+      <c r="AH1" s="1" t="inlineStr">
+        <is>
+          <t>Lois M.</t>
+        </is>
+      </c>
+      <c r="AI1" s="1" t="inlineStr">
+        <is>
+          <t>Lorie M.</t>
+        </is>
+      </c>
+      <c r="AJ1" s="1" t="inlineStr">
+        <is>
+          <t>Marty M.</t>
+        </is>
+      </c>
+      <c r="AK1" s="1" t="inlineStr">
+        <is>
+          <t>Mel W. #1</t>
+        </is>
+      </c>
+      <c r="AL1" s="1" t="inlineStr">
+        <is>
+          <t>Mel W. #2</t>
+        </is>
+      </c>
+      <c r="AM1" s="1" t="inlineStr">
+        <is>
+          <t>Paige P.</t>
+        </is>
+      </c>
+      <c r="AN1" s="1" t="inlineStr">
+        <is>
+          <t>Paul T.</t>
+        </is>
+      </c>
+      <c r="AO1" s="1" t="inlineStr">
+        <is>
+          <t>Preston K.</t>
+        </is>
+      </c>
+      <c r="AP1" s="1" t="inlineStr">
+        <is>
+          <t>Rick S.</t>
+        </is>
+      </c>
+      <c r="AQ1" s="1" t="inlineStr">
+        <is>
+          <t>Reid V.</t>
+        </is>
+      </c>
+      <c r="AR1" s="1" t="inlineStr">
+        <is>
+          <t>Rob S.</t>
+        </is>
+      </c>
+      <c r="AS1" s="1" t="inlineStr">
+        <is>
+          <t>Rod D.</t>
+        </is>
+      </c>
+      <c r="AT1" s="1" t="inlineStr">
+        <is>
+          <t>Ron P.</t>
+        </is>
+      </c>
+      <c r="AU1" s="1" t="inlineStr">
+        <is>
+          <t>Ryan B.</t>
+        </is>
+      </c>
+      <c r="AV1" s="1" t="inlineStr">
+        <is>
+          <t>Sandra P.</t>
+        </is>
+      </c>
+      <c r="AW1" s="1" t="inlineStr">
+        <is>
+          <t>Sal G.</t>
+        </is>
+      </c>
+      <c r="AX1" s="1" t="inlineStr">
+        <is>
+          <t>Sergio E.</t>
+        </is>
+      </c>
+      <c r="AY1" s="1" t="inlineStr">
+        <is>
+          <t>Stacey M.</t>
+        </is>
+      </c>
+      <c r="AZ1" s="1" t="inlineStr">
+        <is>
+          <t>Toni M.</t>
         </is>
       </c>
     </row>
@@ -493,44 +708,259 @@
           <t>1</t>
         </is>
       </c>
-      <c r="B2" s="2" t="inlineStr">
-        <is>
-          <t>KC</t>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>LAR</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>CHI</t>
-        </is>
-      </c>
-      <c r="D2" s="2" t="inlineStr">
-        <is>
-          <t>BAL</t>
-        </is>
-      </c>
-      <c r="E2" s="2" t="inlineStr">
-        <is>
-          <t>SF</t>
+          <t>PIT</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>DEN</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>DEN</t>
         </is>
       </c>
       <c r="F2" s="2" t="inlineStr">
         <is>
-          <t>SF</t>
+          <t>NE</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>LAC</t>
-        </is>
-      </c>
-      <c r="H2" s="2" t="inlineStr">
-        <is>
-          <t>DET</t>
-        </is>
-      </c>
-      <c r="I2" s="2" t="inlineStr">
+          <t>DEN</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>ARI</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>DEN</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>DEN</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
         <is>
           <t>PIT</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>ARI</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>WSH</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>PIT</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>PHI</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>DEN</t>
+        </is>
+      </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>WSH</t>
+        </is>
+      </c>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>ARI</t>
+        </is>
+      </c>
+      <c r="S2" t="inlineStr">
+        <is>
+          <t>DEN</t>
+        </is>
+      </c>
+      <c r="T2" t="inlineStr">
+        <is>
+          <t>ARI</t>
+        </is>
+      </c>
+      <c r="U2" t="inlineStr">
+        <is>
+          <t>LAR</t>
+        </is>
+      </c>
+      <c r="V2" t="inlineStr">
+        <is>
+          <t>CIN</t>
+        </is>
+      </c>
+      <c r="W2" t="inlineStr">
+        <is>
+          <t>ARI</t>
+        </is>
+      </c>
+      <c r="X2" t="inlineStr">
+        <is>
+          <t>PHI</t>
+        </is>
+      </c>
+      <c r="Y2" t="inlineStr">
+        <is>
+          <t>DEN</t>
+        </is>
+      </c>
+      <c r="Z2" s="2" t="inlineStr">
+        <is>
+          <t>MIA</t>
+        </is>
+      </c>
+      <c r="AA2" t="inlineStr">
+        <is>
+          <t>PHI</t>
+        </is>
+      </c>
+      <c r="AB2" t="inlineStr">
+        <is>
+          <t>ARI</t>
+        </is>
+      </c>
+      <c r="AC2" t="inlineStr">
+        <is>
+          <t>DEN</t>
+        </is>
+      </c>
+      <c r="AD2" t="inlineStr">
+        <is>
+          <t>CIN</t>
+        </is>
+      </c>
+      <c r="AE2" t="inlineStr">
+        <is>
+          <t>PIT</t>
+        </is>
+      </c>
+      <c r="AF2" t="inlineStr">
+        <is>
+          <t>DEN</t>
+        </is>
+      </c>
+      <c r="AG2" t="inlineStr">
+        <is>
+          <t>ARI</t>
+        </is>
+      </c>
+      <c r="AH2" t="inlineStr">
+        <is>
+          <t>PHI</t>
+        </is>
+      </c>
+      <c r="AI2" t="inlineStr">
+        <is>
+          <t>DEN</t>
+        </is>
+      </c>
+      <c r="AJ2" t="inlineStr">
+        <is>
+          <t>DEN</t>
+        </is>
+      </c>
+      <c r="AK2" t="inlineStr">
+        <is>
+          <t>DEN</t>
+        </is>
+      </c>
+      <c r="AL2" t="inlineStr">
+        <is>
+          <t>WSH</t>
+        </is>
+      </c>
+      <c r="AM2" t="inlineStr">
+        <is>
+          <t>PHI</t>
+        </is>
+      </c>
+      <c r="AN2" t="inlineStr">
+        <is>
+          <t>ARI</t>
+        </is>
+      </c>
+      <c r="AO2" t="inlineStr">
+        <is>
+          <t>DEN</t>
+        </is>
+      </c>
+      <c r="AP2" t="inlineStr">
+        <is>
+          <t>DEN</t>
+        </is>
+      </c>
+      <c r="AQ2" t="inlineStr">
+        <is>
+          <t>DEN</t>
+        </is>
+      </c>
+      <c r="AR2" t="inlineStr">
+        <is>
+          <t>DEN</t>
+        </is>
+      </c>
+      <c r="AS2" t="inlineStr">
+        <is>
+          <t>WSH</t>
+        </is>
+      </c>
+      <c r="AT2" t="inlineStr">
+        <is>
+          <t>DEN</t>
+        </is>
+      </c>
+      <c r="AU2" t="inlineStr">
+        <is>
+          <t>CIN</t>
+        </is>
+      </c>
+      <c r="AV2" t="inlineStr">
+        <is>
+          <t>WSH</t>
+        </is>
+      </c>
+      <c r="AW2" s="2" t="inlineStr">
+        <is>
+          <t>CLE</t>
+        </is>
+      </c>
+      <c r="AX2" t="inlineStr">
+        <is>
+          <t>WSH</t>
+        </is>
+      </c>
+      <c r="AY2" t="inlineStr">
+        <is>
+          <t>WSH</t>
+        </is>
+      </c>
+      <c r="AZ2" t="inlineStr">
+        <is>
+          <t>WSH</t>
         </is>
       </c>
     </row>
@@ -540,46 +970,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>IND</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>LAC</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>BUF</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>DEN</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>CIN</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>CLE</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>HOU</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>IND</t>
-        </is>
-      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -587,46 +977,6 @@
           <t>3</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>PHI</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>SEA</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>DAL</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>WAS</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>NYJ</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>ARI</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>MIA</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>NYG</t>
-        </is>
-      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -634,46 +984,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>IND</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>NE</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>LAR</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>CAR</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>ATL</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>TEN</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>TB</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>LV</t>
-        </is>
-      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -779,19 +1089,25 @@
           <t>Total</t>
         </is>
       </c>
-      <c r="B20" t="n">
-        <v>1</v>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="D20" t="n">
-        <v>1</v>
-      </c>
-      <c r="E20" t="n">
-        <v>1</v>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
       <c r="F20" t="n">
         <v>1</v>
@@ -801,11 +1117,226 @@
           <t>0</t>
         </is>
       </c>
-      <c r="H20" t="n">
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M20" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N20" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="O20" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="P20" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="Q20" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="R20" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="S20" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="T20" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="U20" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="V20" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="W20" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="X20" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="Y20" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="Z20" t="n">
         <v>1</v>
       </c>
-      <c r="I20" t="n">
+      <c r="AA20" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AB20" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AC20" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AD20" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AE20" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AF20" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AG20" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AH20" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AI20" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AJ20" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AK20" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AL20" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AM20" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AN20" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AO20" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AP20" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AQ20" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AR20" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AS20" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AT20" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AU20" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AV20" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AW20" t="n">
         <v>1</v>
+      </c>
+      <c r="AX20" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AY20" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AZ20" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>